<commit_message>
Cambio en la forma de guardar nuevos archivos: Ahora se puede elegir la ruta.
</commit_message>
<xml_diff>
--- a/Cosas por hacer/Funciones pendientes.xlsx
+++ b/Cosas por hacer/Funciones pendientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicjo\Documents\NetBeansProjects\VicText\Cosas por hacer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B420B88E-D930-4C58-8AE3-15318F2FA493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5458FBB-A4AC-4DCD-B35B-0FE91C500D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D7C35E0-AF02-4AEB-99C3-A81EED4DD625}"/>
+    <workbookView xWindow="6495" yWindow="2205" windowWidth="15705" windowHeight="11250" xr2:uid="{6D7C35E0-AF02-4AEB-99C3-A81EED4DD625}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,13 +56,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,13 +92,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,7 +406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -393,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F2CF481-AEDB-44F1-B26B-0DA95CA09646}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,12 +425,13 @@
     <col min="1" max="1" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>